<commit_message>
added a debug test
</commit_message>
<xml_diff>
--- a/output/amount-of-files.xlsx
+++ b/output/amount-of-files.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/myounes/Documents/Code/thesis/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BDBD46E-5448-3745-B744-9A20C4267136}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20D9E25F-C4C8-3E41-ACEE-0513D07CD190}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-31560" yWindow="600" windowWidth="27920" windowHeight="15900" activeTab="4" xr2:uid="{D995A798-2BBA-3D41-A8D8-5B5A3B8306E5}"/>
+    <workbookView xWindow="-36220" yWindow="680" windowWidth="27920" windowHeight="15900" activeTab="4" xr2:uid="{D995A798-2BBA-3D41-A8D8-5B5A3B8306E5}"/>
   </bookViews>
   <sheets>
     <sheet name="50files" sheetId="2" r:id="rId1"/>
@@ -2789,204 +2789,282 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'500files'!$C$1:$C$65</c:f>
+              <c:f>'500files'!$C$1:$C$101</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="65"/>
+                <c:ptCount val="101"/>
                 <c:pt idx="0">
-                  <c:v>23.928144454956001</c:v>
+                  <c:v>25.365270614623999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25.1916179656982</c:v>
+                  <c:v>23.431138992309499</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24.5269470214843</c:v>
+                  <c:v>22.251497268676701</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>23.269462585449201</c:v>
+                  <c:v>22.4071865081787</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>24.592815399169901</c:v>
+                  <c:v>23.3772468566894</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>25.1856288909912</c:v>
+                  <c:v>24.113773345947202</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>22.622755050659102</c:v>
+                  <c:v>22.820360183715799</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>24.1736526489257</c:v>
+                  <c:v>23.347307205200099</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>23.419162750244102</c:v>
+                  <c:v>23.1377258300781</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>22.7305393218994</c:v>
+                  <c:v>22.712575912475501</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>22.9161682128906</c:v>
+                  <c:v>22.497007369995099</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>23.0718574523925</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>23.089820861816399</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>23.389223098754801</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>22.8682651519775</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>23.706586837768501</c:v>
                 </c:pt>
-                <c:pt idx="12">
-                  <c:v>22.8802394866943</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>23.371257781982401</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>22.820360183715799</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>23.179641723632798</c:v>
-                </c:pt>
                 <c:pt idx="16">
-                  <c:v>24.329341888427699</c:v>
+                  <c:v>24.335330963134702</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>23.149702072143501</c:v>
+                  <c:v>23.3053894042968</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>24.724552154541001</c:v>
+                  <c:v>24.652694702148398</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>24.532934188842699</c:v>
+                  <c:v>25.1017971038818</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>23.047904968261701</c:v>
+                  <c:v>23.6287441253662</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>24.347307205200099</c:v>
+                  <c:v>25.688623428344702</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>25.083833694458001</c:v>
+                  <c:v>25.125749588012599</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>25.742515563964801</c:v>
+                  <c:v>25.1017971038818</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>24.712575912475501</c:v>
+                  <c:v>25.131736755371001</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>24.700599670410099</c:v>
+                  <c:v>24.898204803466701</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>25.598802566528299</c:v>
+                  <c:v>25.215570449829102</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>26.275449752807599</c:v>
+                  <c:v>24.7485046386718</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>25.6287441253662</c:v>
+                  <c:v>24.754491806030199</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>27.119762420654201</c:v>
+                  <c:v>27.353294372558501</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>24.712575912475501</c:v>
+                  <c:v>24.844312667846602</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>24.131736755371001</c:v>
+                  <c:v>24.083833694458001</c:v>
                 </c:pt>
                 <c:pt idx="32">
                   <c:v>26.449102401733398</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>26.520959854125898</c:v>
+                  <c:v>26.311378479003899</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>27.467067718505799</c:v>
+                  <c:v>26.1077861785888</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>25.676647186279201</c:v>
+                  <c:v>25.4071865081787</c:v>
                 </c:pt>
                 <c:pt idx="36">
+                  <c:v>25.9880256652832</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>26.431138992309499</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>26.149702072143501</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>26.694612503051701</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>25.694612503051701</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>24.712575912475501</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>25.7305393218994</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>26.011976242065401</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>25.538923263549801</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>25.550899505615199</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>24.598802566528299</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>25.3592815399169</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>25.443115234375</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>25.826347351074201</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>26.778444290161101</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>25.479042053222599</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>25.2574863433837</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>25.910181045532202</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>24.964073181152301</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>25.473054885864201</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>25.778444290161101</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>27.143712997436499</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>25.467067718505799</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>24.994012832641602</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>25.856288909912099</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>24.658683776855401</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>25.083833694458001</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>24.784431457519499</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>25.2395210266113</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>25.3053894042968</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>25.712575912475501</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>24.910181045532202</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>24.760480880737301</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>25.1736545562744</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>24.796407699584901</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>24.497007369995099</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>24.688623428344702</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>24.964073181152301</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>27.556886672973601</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>25.904191970825099</c:v>
+                </c:pt>
+                <c:pt idx="76">
                   <c:v>25.850299835205</c:v>
                 </c:pt>
-                <c:pt idx="37">
-                  <c:v>26.275449752807599</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>26.389223098754801</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>27.2215576171875</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>25.0718574523925</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>25.1556892395019</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>25.964073181152301</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>26.143712997436499</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>25.041917800903299</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>25.245510101318299</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>24.233533859252901</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>25.1077861785888</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>25.215570449829102</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>25.263473510742099</c:v>
-                </c:pt>
-                <c:pt idx="50">
+                <c:pt idx="77">
+                  <c:v>26.179641723632798</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>27.131736755371001</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>25.125749588012599</c:v>
+                </c:pt>
+                <c:pt idx="80">
                   <c:v>25.856288909912099</c:v>
                 </c:pt>
-                <c:pt idx="51">
-                  <c:v>25.4071865081787</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>25.113773345947202</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>26.592815399169901</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>25.706586837768501</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>25.2574863433837</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>25.784431457519499</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>26.065868377685501</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>25.5269470214843</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>25.479042053222599</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>26.3592815399169</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>24.7305393218994</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>25.3053894042968</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>25.371257781982401</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>25.215570449829102</c:v>
+                <c:pt idx="81">
+                  <c:v>26.011976242065401</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>25.0359287261962</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>26.1556892395019</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>25.0538940429687</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>25.497007369995099</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>24.293413162231399</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>26.772455215454102</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>25.8023967742919</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>27.179641723632798</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>25.3413181304931</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3018,204 +3096,282 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'500files'!$B$1:$B$65</c:f>
+              <c:f>'500files'!$B$1:$B$101</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="65"/>
+                <c:ptCount val="101"/>
                 <c:pt idx="0">
-                  <c:v>24.737804412841701</c:v>
+                  <c:v>24.7073154449462</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>26.213413238525298</c:v>
+                  <c:v>25.6463413238525</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>27.993902206420898</c:v>
+                  <c:v>29.262193679809499</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30.951217651367099</c:v>
+                  <c:v>31.493902206420898</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>32.329265594482401</c:v>
+                  <c:v>32.445121765136697</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>33.414634704589801</c:v>
+                  <c:v>33.396339416503899</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>33.591461181640597</c:v>
+                  <c:v>34.182926177978501</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>34.981704711913999</c:v>
+                  <c:v>34.932926177978501</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>36.682926177978501</c:v>
+                  <c:v>35.689022064208899</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>36.329265594482401</c:v>
+                  <c:v>37.5609741210937</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>37.670730590820298</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>38.475608825683501</c:v>
+                  <c:v>37.426826477050703</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>39.079265594482401</c:v>
+                  <c:v>37.451217651367102</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>38.8719482421875</c:v>
+                  <c:v>38.012195587158203</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>40.298778533935497</c:v>
+                  <c:v>41.1646308898925</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>41.359752655029297</c:v>
+                  <c:v>41.1219482421875</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>42.420730590820298</c:v>
+                  <c:v>43.140243530273402</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44.3109741210937</c:v>
+                  <c:v>43.3719482421875</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>43.640243530273402</c:v>
+                  <c:v>43.890243530273402</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>45.951217651367102</c:v>
+                  <c:v>45.939022064208899</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>45.432926177978501</c:v>
+                  <c:v>45.463413238525298</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>46.969509124755803</c:v>
+                  <c:v>47.756095886230398</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>50.012191772460902</c:v>
+                  <c:v>48.774387359619098</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>49.707313537597599</c:v>
+                  <c:v>48.3109741210937</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>50.542682647705</c:v>
+                  <c:v>50.939022064208899</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>52.067070007324197</c:v>
+                  <c:v>51.829265594482401</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>51.201217651367102</c:v>
+                  <c:v>50.682926177978501</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>52.878047943115199</c:v>
+                  <c:v>51.865852355957003</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>53.012191772460902</c:v>
+                  <c:v>53.390243530273402</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>55.384143829345703</c:v>
+                  <c:v>55.262191772460902</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>56.140243530273402</c:v>
+                  <c:v>55.670730590820298</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>56.054874420166001</c:v>
+                  <c:v>55.609752655029297</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>57.402435302734297</c:v>
+                  <c:v>55.6646308898925</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>57.963413238525298</c:v>
+                  <c:v>57.737804412841797</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>56.896339416503899</c:v>
+                  <c:v>57.042682647705</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>57.890243530273402</c:v>
+                  <c:v>57.707313537597599</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>60.597557067871001</c:v>
+                  <c:v>58.451217651367102</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>59.463413238525298</c:v>
+                  <c:v>59.445117950439403</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>61.384143829345703</c:v>
+                  <c:v>59.646339416503899</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>60.975608825683501</c:v>
+                  <c:v>61.506095886230398</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>61.432926177978501</c:v>
+                  <c:v>60.585365295410099</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>62.774387359619098</c:v>
+                  <c:v>61.085365295410099</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>61.628047943115199</c:v>
+                  <c:v>62.3536567687988</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>63.1036567687988</c:v>
+                  <c:v>62.207313537597599</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>63.012191772460902</c:v>
+                  <c:v>62.713413238525298</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>63.073169708251903</c:v>
+                  <c:v>63.054874420166001</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>64.804878234863196</c:v>
+                  <c:v>62.3109741210937</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>63.536582946777301</c:v>
+                  <c:v>62.262191772460902</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>63.817070007324197</c:v>
+                  <c:v>64.414634704589801</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>65.164634704589801</c:v>
+                  <c:v>63.512191772460902</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>66.615852355957003</c:v>
+                  <c:v>64.390243530273395</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>65.439018249511705</c:v>
+                  <c:v>65.091461181640597</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>65.25</c:v>
+                  <c:v>64.609756469726506</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>66.981704711914006</c:v>
+                  <c:v>64.890243530273395</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>66.207313537597599</c:v>
+                  <c:v>64.798774719238196</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>65.756095886230398</c:v>
+                  <c:v>65.189018249511705</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>66.091461181640597</c:v>
+                  <c:v>66.323165893554602</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>66.189018249511705</c:v>
+                  <c:v>66.402435302734304</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>67.475608825683594</c:v>
+                  <c:v>64.664634704589801</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>66.451217651367102</c:v>
+                  <c:v>67.585365295410099</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>66.993896484375</c:v>
+                  <c:v>65.713409423828097</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>66.908531188964801</c:v>
+                  <c:v>66.518287658691406</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>67.725608825683594</c:v>
+                  <c:v>67.060974121093693</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>67.689018249511705</c:v>
+                  <c:v>67.628044128417898</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>68.682922363281193</c:v>
+                  <c:v>66.939018249511705</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>67.25</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>68.201217651367102</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>68.689018249511705</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>69.896339416503906</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>70.353652954101506</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>70.560974121093693</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>70.012191772460895</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>70.963409423828097</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>70.317070007324205</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>70.408531188964801</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>72.243896484375</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>71.189018249511705</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>72.262191772460895</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>71.579269409179602</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>72.695121765136705</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>71.524391174316406</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>72.292678833007798</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>72.164634704589801</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>72.274391174316406</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>73.628044128417898</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>72.091461181640597</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>73.347557067871094</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>72.487800598144503</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>73.109756469726506</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>73.664634704589801</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>74.1219482421875</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8371,10 +8527,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F87E5C3-EEAD-A44E-A86A-801C73B6171A}">
-  <dimension ref="A1:E65"/>
+  <dimension ref="A1:E91"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection sqref="A1:E91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8384,16 +8540,16 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <v>24.737804412841701</v>
+        <v>24.7073154449462</v>
       </c>
       <c r="C1">
-        <v>23.928144454956001</v>
+        <v>25.365270614623999</v>
       </c>
       <c r="D1">
-        <v>0.69707530736923196</v>
+        <v>0.69407898187637296</v>
       </c>
       <c r="E1">
-        <v>1.3907158374786299</v>
+        <v>1.3913315534591599</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -8401,16 +8557,16 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>26.213413238525298</v>
+        <v>25.6463413238525</v>
       </c>
       <c r="C2">
-        <v>25.1916179656982</v>
+        <v>23.431138992309499</v>
       </c>
       <c r="D2">
-        <v>0.69365197420120195</v>
+        <v>0.69228112697601296</v>
       </c>
       <c r="E2">
-        <v>1.3874135017395</v>
+        <v>1.3901168107986399</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -8418,16 +8574,16 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>27.993902206420898</v>
+        <v>29.262193679809499</v>
       </c>
       <c r="C3">
-        <v>24.5269470214843</v>
+        <v>22.251497268676701</v>
       </c>
       <c r="D3">
-        <v>0.69021266698837203</v>
+        <v>0.690315842628479</v>
       </c>
       <c r="E3">
-        <v>1.3886792659759499</v>
+        <v>1.3906338214874201</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -8435,16 +8591,16 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>30.951217651367099</v>
+        <v>31.493902206420898</v>
       </c>
       <c r="C4">
-        <v>23.269462585449201</v>
+        <v>22.4071865081787</v>
       </c>
       <c r="D4">
-        <v>0.68783146142959595</v>
+        <v>0.688160359859466</v>
       </c>
       <c r="E4">
-        <v>1.3898800611495901</v>
+        <v>1.3917754888534499</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -8452,16 +8608,16 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>32.329265594482401</v>
+        <v>32.445121765136697</v>
       </c>
       <c r="C5">
-        <v>24.592815399169901</v>
+        <v>23.3772468566894</v>
       </c>
       <c r="D5">
-        <v>0.68464726209640503</v>
+        <v>0.68462008237838701</v>
       </c>
       <c r="E5">
-        <v>1.3907111883163401</v>
+        <v>1.3937170505523599</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -8469,16 +8625,16 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>33.414634704589801</v>
+        <v>33.396339416503899</v>
       </c>
       <c r="C6">
-        <v>25.1856288909912</v>
+        <v>24.113773345947202</v>
       </c>
       <c r="D6">
-        <v>0.68122524023055997</v>
+        <v>0.68234181404113703</v>
       </c>
       <c r="E6">
-        <v>1.3930416107177701</v>
+        <v>1.3954260349273599</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -8486,16 +8642,16 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>33.591461181640597</v>
+        <v>34.182926177978501</v>
       </c>
       <c r="C7">
-        <v>22.622755050659102</v>
+        <v>22.820360183715799</v>
       </c>
       <c r="D7">
-        <v>0.67850142717361395</v>
+        <v>0.67867583036422696</v>
       </c>
       <c r="E7">
-        <v>1.40360939502716</v>
+        <v>1.4056481122970499</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -8503,16 +8659,16 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>34.981704711913999</v>
+        <v>34.932926177978501</v>
       </c>
       <c r="C8">
-        <v>24.1736526489257</v>
+        <v>23.347307205200099</v>
       </c>
       <c r="D8">
-        <v>0.67510926723480202</v>
+        <v>0.67488753795623702</v>
       </c>
       <c r="E8">
-        <v>1.40078485012054</v>
+        <v>1.40547275543212</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -8520,16 +8676,16 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>36.682926177978501</v>
+        <v>35.689022064208899</v>
       </c>
       <c r="C9">
-        <v>23.419162750244102</v>
+        <v>23.1377258300781</v>
       </c>
       <c r="D9">
-        <v>0.66992783546447698</v>
+        <v>0.67082029581069902</v>
       </c>
       <c r="E9">
-        <v>1.40876817703247</v>
+        <v>1.41097724437713</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -8537,16 +8693,16 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>36.329265594482401</v>
+        <v>37.5609741210937</v>
       </c>
       <c r="C10">
-        <v>22.7305393218994</v>
+        <v>22.712575912475501</v>
       </c>
       <c r="D10">
-        <v>0.66619187593460005</v>
+        <v>0.66342771053314198</v>
       </c>
       <c r="E10">
-        <v>1.42106580734252</v>
+        <v>1.4307551383972099</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -8557,13 +8713,13 @@
         <v>37.670730590820298</v>
       </c>
       <c r="C11">
-        <v>22.9161682128906</v>
+        <v>22.497007369995099</v>
       </c>
       <c r="D11">
-        <v>0.66150814294814997</v>
+        <v>0.66224926710128695</v>
       </c>
       <c r="E11">
-        <v>1.44398701190948</v>
+        <v>1.4438620805740301</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -8571,16 +8727,16 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>38.475608825683501</v>
+        <v>37.426826477050703</v>
       </c>
       <c r="C12">
-        <v>23.706586837768501</v>
+        <v>23.0718574523925</v>
       </c>
       <c r="D12">
-        <v>0.65508013963699296</v>
+        <v>0.65670496225357</v>
       </c>
       <c r="E12">
-        <v>1.4547134637832599</v>
+        <v>1.4544694423675499</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -8588,16 +8744,16 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>39.079265594482401</v>
+        <v>37.451217651367102</v>
       </c>
       <c r="C13">
-        <v>22.8802394866943</v>
+        <v>23.089820861816399</v>
       </c>
       <c r="D13">
-        <v>0.65301197767257602</v>
+        <v>0.65232795476913397</v>
       </c>
       <c r="E13">
-        <v>1.4950242042541499</v>
+        <v>1.4841948747634801</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -8605,16 +8761,16 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>38.8719482421875</v>
+        <v>38.012195587158203</v>
       </c>
       <c r="C14">
-        <v>23.371257781982401</v>
+        <v>23.389223098754801</v>
       </c>
       <c r="D14">
-        <v>0.64781117439269997</v>
+        <v>0.64949631690979004</v>
       </c>
       <c r="E14">
-        <v>1.4927847385406401</v>
+        <v>1.4872730970382599</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -8622,16 +8778,16 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>40.298778533935497</v>
+        <v>41.1646308898925</v>
       </c>
       <c r="C15">
-        <v>22.820360183715799</v>
+        <v>22.8682651519775</v>
       </c>
       <c r="D15">
-        <v>0.643293857574462</v>
+        <v>0.639265596866607</v>
       </c>
       <c r="E15">
-        <v>1.5255869626998899</v>
+        <v>1.53661131858825</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -8639,16 +8795,16 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>41.359752655029297</v>
+        <v>41.1219482421875</v>
       </c>
       <c r="C16">
-        <v>23.179641723632798</v>
+        <v>23.706586837768501</v>
       </c>
       <c r="D16">
-        <v>0.63397729396820002</v>
+        <v>0.634330093860626</v>
       </c>
       <c r="E16">
-        <v>1.5541037321090601</v>
+        <v>1.54905700683593</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -8656,16 +8812,16 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>42.420730590820298</v>
+        <v>43.140243530273402</v>
       </c>
       <c r="C17">
-        <v>24.329341888427699</v>
+        <v>24.335330963134702</v>
       </c>
       <c r="D17">
-        <v>0.62846416234970004</v>
+        <v>0.62823575735092096</v>
       </c>
       <c r="E17">
-        <v>1.5905523300170801</v>
+        <v>1.5847810506820601</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -8673,16 +8829,16 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>44.3109741210937</v>
+        <v>43.3719482421875</v>
       </c>
       <c r="C18">
-        <v>23.149702072143501</v>
+        <v>23.3053894042968</v>
       </c>
       <c r="D18">
-        <v>0.62386184930801303</v>
+        <v>0.62231969833374001</v>
       </c>
       <c r="E18">
-        <v>1.6492216587066599</v>
+        <v>1.64183461666107</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -8690,16 +8846,16 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>43.640243530273402</v>
+        <v>43.890243530273402</v>
       </c>
       <c r="C19">
-        <v>24.724552154541001</v>
+        <v>24.652694702148398</v>
       </c>
       <c r="D19">
-        <v>0.61795860528945901</v>
+        <v>0.61448371410369795</v>
       </c>
       <c r="E19">
-        <v>1.6032123565673799</v>
+        <v>1.64817702770233</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -8707,16 +8863,16 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>45.951217651367102</v>
+        <v>45.939022064208899</v>
       </c>
       <c r="C20">
-        <v>24.532934188842699</v>
+        <v>25.1017971038818</v>
       </c>
       <c r="D20">
-        <v>0.61150330305099398</v>
+        <v>0.60694628953933705</v>
       </c>
       <c r="E20">
-        <v>1.61895883083343</v>
+        <v>1.6673568487167301</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -8724,16 +8880,16 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>45.432926177978501</v>
+        <v>45.463413238525298</v>
       </c>
       <c r="C21">
-        <v>23.047904968261701</v>
+        <v>23.6287441253662</v>
       </c>
       <c r="D21">
-        <v>0.60385739803314198</v>
+        <v>0.60315352678298895</v>
       </c>
       <c r="E21">
-        <v>1.69632256031036</v>
+        <v>1.7268157005310001</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -8741,16 +8897,16 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>46.969509124755803</v>
+        <v>47.756095886230398</v>
       </c>
       <c r="C22">
-        <v>24.347307205200099</v>
+        <v>25.688623428344702</v>
       </c>
       <c r="D22">
-        <v>0.59487557411193803</v>
+        <v>0.59195476770401001</v>
       </c>
       <c r="E22">
-        <v>1.68987584114074</v>
+        <v>1.74893033504486</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -8758,16 +8914,16 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>50.012191772460902</v>
+        <v>48.774387359619098</v>
       </c>
       <c r="C23">
-        <v>25.083833694458001</v>
+        <v>25.125749588012599</v>
       </c>
       <c r="D23">
-        <v>0.58318352699279696</v>
+        <v>0.58672314882278398</v>
       </c>
       <c r="E23">
-        <v>1.82282090187072</v>
+        <v>1.8886864185333201</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -8775,16 +8931,16 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>49.707313537597599</v>
+        <v>48.3109741210937</v>
       </c>
       <c r="C24">
-        <v>25.742515563964801</v>
+        <v>25.1017971038818</v>
       </c>
       <c r="D24">
-        <v>0.58162671327590898</v>
+        <v>0.58157759904861395</v>
       </c>
       <c r="E24">
-        <v>1.7265446186065601</v>
+        <v>1.7947348356246899</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -8792,16 +8948,16 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>50.542682647705</v>
+        <v>50.939022064208899</v>
       </c>
       <c r="C25">
-        <v>24.712575912475501</v>
+        <v>25.131736755371001</v>
       </c>
       <c r="D25">
-        <v>0.57656556367874101</v>
+        <v>0.573963522911071</v>
       </c>
       <c r="E25">
-        <v>1.8174306154251001</v>
+        <v>1.8904736042022701</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -8809,16 +8965,16 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>52.067070007324197</v>
+        <v>51.829265594482401</v>
       </c>
       <c r="C26">
-        <v>24.700599670410099</v>
+        <v>24.898204803466701</v>
       </c>
       <c r="D26">
-        <v>0.56597584486007602</v>
+        <v>0.56413650512695301</v>
       </c>
       <c r="E26">
-        <v>1.83688676357269</v>
+        <v>1.89537978172302</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -8826,16 +8982,16 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>51.201217651367102</v>
+        <v>50.682926177978501</v>
       </c>
       <c r="C27">
-        <v>25.598802566528299</v>
+        <v>25.215570449829102</v>
       </c>
       <c r="D27">
-        <v>0.56426537036895696</v>
+        <v>0.56344783306121804</v>
       </c>
       <c r="E27">
-        <v>2.02519631385803</v>
+        <v>2.0137014389038002</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -8843,16 +8999,16 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>52.878047943115199</v>
+        <v>51.865852355957003</v>
       </c>
       <c r="C28">
-        <v>26.275449752807599</v>
+        <v>24.7485046386718</v>
       </c>
       <c r="D28">
-        <v>0.55614626407623202</v>
+        <v>0.55500525236129705</v>
       </c>
       <c r="E28">
-        <v>1.9836112260818399</v>
+        <v>2.08548736572265</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -8860,16 +9016,16 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>53.012191772460902</v>
+        <v>53.390243530273402</v>
       </c>
       <c r="C29">
-        <v>25.6287441253662</v>
+        <v>24.754491806030199</v>
       </c>
       <c r="D29">
-        <v>0.55070191621780396</v>
+        <v>0.54847085475921598</v>
       </c>
       <c r="E29">
-        <v>2.1141285896301198</v>
+        <v>2.1432530879974299</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -8877,16 +9033,16 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>55.384143829345703</v>
+        <v>55.262191772460902</v>
       </c>
       <c r="C30">
-        <v>27.119762420654201</v>
+        <v>27.353294372558501</v>
       </c>
       <c r="D30">
-        <v>0.537242472171783</v>
+        <v>0.54109871387481601</v>
       </c>
       <c r="E30">
-        <v>2.02778792381286</v>
+        <v>2.0627782344818102</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
@@ -8894,16 +9050,16 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>56.140243530273402</v>
+        <v>55.670730590820298</v>
       </c>
       <c r="C31">
-        <v>24.712575912475501</v>
+        <v>24.844312667846602</v>
       </c>
       <c r="D31">
-        <v>0.53441423177719105</v>
+        <v>0.531344413757324</v>
       </c>
       <c r="E31">
-        <v>2.0579133033752401</v>
+        <v>2.2406837940215998</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
@@ -8911,16 +9067,16 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <v>56.054874420166001</v>
+        <v>55.609752655029297</v>
       </c>
       <c r="C32">
-        <v>24.131736755371001</v>
+        <v>24.083833694458001</v>
       </c>
       <c r="D32">
-        <v>0.52600324153900102</v>
+        <v>0.52842271327972401</v>
       </c>
       <c r="E32">
-        <v>2.1950309276580802</v>
+        <v>2.2746415138244598</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
@@ -8928,16 +9084,16 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <v>57.402435302734297</v>
+        <v>55.6646308898925</v>
       </c>
       <c r="C33">
         <v>26.449102401733398</v>
       </c>
       <c r="D33">
-        <v>0.51841723918914795</v>
+        <v>0.520247042179107</v>
       </c>
       <c r="E33">
-        <v>2.1611292362213099</v>
+        <v>2.26891613006591</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
@@ -8945,16 +9101,16 @@
         <v>33</v>
       </c>
       <c r="B34">
-        <v>57.963413238525298</v>
+        <v>57.737804412841797</v>
       </c>
       <c r="C34">
-        <v>26.520959854125898</v>
+        <v>26.311378479003899</v>
       </c>
       <c r="D34">
-        <v>0.51766997575759799</v>
+        <v>0.51407319307327204</v>
       </c>
       <c r="E34">
-        <v>2.2717537879943799</v>
+        <v>2.3882210254669101</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
@@ -8962,16 +9118,16 @@
         <v>34</v>
       </c>
       <c r="B35">
-        <v>56.896339416503899</v>
+        <v>57.042682647705</v>
       </c>
       <c r="C35">
-        <v>27.467067718505799</v>
+        <v>26.1077861785888</v>
       </c>
       <c r="D35">
-        <v>0.50857681035995395</v>
+        <v>0.51021683216094904</v>
       </c>
       <c r="E35">
-        <v>2.2527213096618599</v>
+        <v>2.2134156227111799</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
@@ -8979,16 +9135,16 @@
         <v>35</v>
       </c>
       <c r="B36">
-        <v>57.890243530273402</v>
+        <v>57.707313537597599</v>
       </c>
       <c r="C36">
-        <v>25.676647186279201</v>
+        <v>25.4071865081787</v>
       </c>
       <c r="D36">
-        <v>0.50668913125991799</v>
+        <v>0.50811254978179898</v>
       </c>
       <c r="E36">
-        <v>2.1048943996429399</v>
+        <v>2.2772843837738002</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
@@ -8996,16 +9152,16 @@
         <v>36</v>
       </c>
       <c r="B37">
-        <v>60.597557067871001</v>
+        <v>58.451217651367102</v>
       </c>
       <c r="C37">
-        <v>25.850299835205</v>
+        <v>25.9880256652832</v>
       </c>
       <c r="D37">
-        <v>0.49384129047393799</v>
+        <v>0.49875786900520303</v>
       </c>
       <c r="E37">
-        <v>2.6634178161621</v>
+        <v>2.9064157009124698</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
@@ -9013,16 +9169,16 @@
         <v>37</v>
       </c>
       <c r="B38">
-        <v>59.463413238525298</v>
+        <v>59.445117950439403</v>
       </c>
       <c r="C38">
-        <v>26.275449752807599</v>
+        <v>26.431138992309499</v>
       </c>
       <c r="D38">
-        <v>0.492344349622726</v>
+        <v>0.49018782377242998</v>
       </c>
       <c r="E38">
-        <v>2.7589650154113698</v>
+        <v>2.7101418972015301</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
@@ -9030,16 +9186,16 @@
         <v>38</v>
       </c>
       <c r="B39">
-        <v>61.384143829345703</v>
+        <v>59.646339416503899</v>
       </c>
       <c r="C39">
-        <v>26.389223098754801</v>
+        <v>26.149702072143501</v>
       </c>
       <c r="D39">
-        <v>0.48107141256332397</v>
+        <v>0.48599129915237399</v>
       </c>
       <c r="E39">
-        <v>2.4960150718688898</v>
+        <v>2.7179510593414302</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
@@ -9047,16 +9203,16 @@
         <v>39</v>
       </c>
       <c r="B40">
-        <v>60.975608825683501</v>
+        <v>61.506095886230398</v>
       </c>
       <c r="C40">
-        <v>27.2215576171875</v>
+        <v>26.694612503051701</v>
       </c>
       <c r="D40">
-        <v>0.480131596326828</v>
+        <v>0.484393030405044</v>
       </c>
       <c r="E40">
-        <v>2.4122252464294398</v>
+        <v>2.70161652565002</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
@@ -9064,16 +9220,16 @@
         <v>40</v>
       </c>
       <c r="B41">
-        <v>61.432926177978501</v>
+        <v>60.585365295410099</v>
       </c>
       <c r="C41">
-        <v>25.0718574523925</v>
+        <v>25.694612503051701</v>
       </c>
       <c r="D41">
-        <v>0.48165914416313099</v>
+        <v>0.47869998216629001</v>
       </c>
       <c r="E41">
-        <v>2.65030741691589</v>
+        <v>2.8246257305145201</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
@@ -9081,16 +9237,16 @@
         <v>41</v>
       </c>
       <c r="B42">
-        <v>62.774387359619098</v>
+        <v>61.085365295410099</v>
       </c>
       <c r="C42">
-        <v>25.1556892395019</v>
+        <v>24.712575912475501</v>
       </c>
       <c r="D42">
-        <v>0.47341722249984702</v>
+        <v>0.47851189970970098</v>
       </c>
       <c r="E42">
-        <v>2.8028659820556601</v>
+        <v>2.8171873092651301</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
@@ -9098,16 +9254,16 @@
         <v>42</v>
       </c>
       <c r="B43">
-        <v>61.628047943115199</v>
+        <v>62.3536567687988</v>
       </c>
       <c r="C43">
-        <v>25.964073181152301</v>
+        <v>25.7305393218994</v>
       </c>
       <c r="D43">
-        <v>0.47248637676239003</v>
+        <v>0.47168231010437001</v>
       </c>
       <c r="E43">
-        <v>2.8810889720916699</v>
+        <v>2.98336458206176</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
@@ -9115,16 +9271,16 @@
         <v>43</v>
       </c>
       <c r="B44">
-        <v>63.1036567687988</v>
+        <v>62.207313537597599</v>
       </c>
       <c r="C44">
-        <v>26.143712997436499</v>
+        <v>26.011976242065401</v>
       </c>
       <c r="D44">
-        <v>0.46110481023788402</v>
+        <v>0.46681582927703802</v>
       </c>
       <c r="E44">
-        <v>2.76766014099121</v>
+        <v>2.7322759628295898</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
@@ -9132,16 +9288,16 @@
         <v>44</v>
       </c>
       <c r="B45">
-        <v>63.012191772460902</v>
+        <v>62.713413238525298</v>
       </c>
       <c r="C45">
-        <v>25.041917800903299</v>
+        <v>25.538923263549801</v>
       </c>
       <c r="D45">
-        <v>0.463377445936203</v>
+        <v>0.45818081498146002</v>
       </c>
       <c r="E45">
-        <v>2.9802286624908398</v>
+        <v>3.4614174365997301</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
@@ -9149,16 +9305,16 @@
         <v>45</v>
       </c>
       <c r="B46">
-        <v>63.073169708251903</v>
+        <v>63.054874420166001</v>
       </c>
       <c r="C46">
-        <v>25.245510101318299</v>
+        <v>25.550899505615199</v>
       </c>
       <c r="D46">
-        <v>0.45617577433586098</v>
+        <v>0.46134138107299799</v>
       </c>
       <c r="E46">
-        <v>3.0099861621856601</v>
+        <v>3.1542170047760001</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
@@ -9166,16 +9322,16 @@
         <v>46</v>
       </c>
       <c r="B47">
-        <v>64.804878234863196</v>
+        <v>62.3109741210937</v>
       </c>
       <c r="C47">
-        <v>24.233533859252901</v>
+        <v>24.598802566528299</v>
       </c>
       <c r="D47">
-        <v>0.45580321550369202</v>
+        <v>0.46411922574043202</v>
       </c>
       <c r="E47">
-        <v>2.7618818283081001</v>
+        <v>3.0049266815185498</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
@@ -9183,16 +9339,16 @@
         <v>47</v>
       </c>
       <c r="B48">
-        <v>63.536582946777301</v>
+        <v>62.262191772460902</v>
       </c>
       <c r="C48">
-        <v>25.1077861785888</v>
+        <v>25.3592815399169</v>
       </c>
       <c r="D48">
-        <v>0.45107504725456199</v>
+        <v>0.45363444089889499</v>
       </c>
       <c r="E48">
-        <v>2.7553341388702299</v>
+        <v>2.9408648014068599</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
@@ -9200,16 +9356,16 @@
         <v>48</v>
       </c>
       <c r="B49">
-        <v>63.817070007324197</v>
+        <v>64.414634704589801</v>
       </c>
       <c r="C49">
-        <v>25.215570449829102</v>
+        <v>25.443115234375</v>
       </c>
       <c r="D49">
-        <v>0.44825705885887102</v>
+        <v>0.45255813002586298</v>
       </c>
       <c r="E49">
-        <v>3.2168917655944802</v>
+        <v>3.3472580909728999</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
@@ -9217,16 +9373,16 @@
         <v>49</v>
       </c>
       <c r="B50">
-        <v>65.164634704589801</v>
+        <v>63.512191772460902</v>
       </c>
       <c r="C50">
-        <v>25.263473510742099</v>
+        <v>25.826347351074201</v>
       </c>
       <c r="D50">
-        <v>0.437709361314773</v>
+        <v>0.45519822835922202</v>
       </c>
       <c r="E50">
-        <v>3.1492507457733101</v>
+        <v>3.0090949535369802</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
@@ -9234,16 +9390,16 @@
         <v>50</v>
       </c>
       <c r="B51">
-        <v>66.615852355957003</v>
+        <v>64.390243530273395</v>
       </c>
       <c r="C51">
-        <v>25.856288909912099</v>
+        <v>26.778444290161101</v>
       </c>
       <c r="D51">
-        <v>0.43882945179939198</v>
+        <v>0.44211575388908297</v>
       </c>
       <c r="E51">
-        <v>3.0051512718200599</v>
+        <v>2.7699491977691602</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
@@ -9251,16 +9407,16 @@
         <v>51</v>
       </c>
       <c r="B52">
-        <v>65.439018249511705</v>
+        <v>65.091461181640597</v>
       </c>
       <c r="C52">
-        <v>25.4071865081787</v>
+        <v>25.479042053222599</v>
       </c>
       <c r="D52">
-        <v>0.43921813368797302</v>
+        <v>0.44479572772979697</v>
       </c>
       <c r="E52">
-        <v>3.1104636192321702</v>
+        <v>2.7967662811279199</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
@@ -9268,16 +9424,16 @@
         <v>52</v>
       </c>
       <c r="B53">
-        <v>65.25</v>
+        <v>64.609756469726506</v>
       </c>
       <c r="C53">
-        <v>25.113773345947202</v>
+        <v>25.2574863433837</v>
       </c>
       <c r="D53">
-        <v>0.43326511979103</v>
+        <v>0.44090926647186202</v>
       </c>
       <c r="E53">
-        <v>3.2430932521820002</v>
+        <v>3.0253312587738002</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
@@ -9285,16 +9441,16 @@
         <v>53</v>
       </c>
       <c r="B54">
-        <v>66.981704711914006</v>
+        <v>64.890243530273395</v>
       </c>
       <c r="C54">
-        <v>26.592815399169901</v>
+        <v>25.910181045532202</v>
       </c>
       <c r="D54">
-        <v>0.43340024352073597</v>
+        <v>0.439308851957321</v>
       </c>
       <c r="E54">
-        <v>3.1928076744079501</v>
+        <v>3.0331926345825102</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
@@ -9302,16 +9458,16 @@
         <v>54</v>
       </c>
       <c r="B55">
-        <v>66.207313537597599</v>
+        <v>64.798774719238196</v>
       </c>
       <c r="C55">
-        <v>25.706586837768501</v>
+        <v>24.964073181152301</v>
       </c>
       <c r="D55">
-        <v>0.42471534013748102</v>
+        <v>0.43697565793991</v>
       </c>
       <c r="E55">
-        <v>3.6636729240417401</v>
+        <v>3.3436682224273602</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
@@ -9319,16 +9475,16 @@
         <v>55</v>
       </c>
       <c r="B56">
-        <v>65.756095886230398</v>
+        <v>65.189018249511705</v>
       </c>
       <c r="C56">
-        <v>25.2574863433837</v>
+        <v>25.473054885864201</v>
       </c>
       <c r="D56">
-        <v>0.43054914474487299</v>
+        <v>0.432375907897949</v>
       </c>
       <c r="E56">
-        <v>3.1712241172790501</v>
+        <v>3.15142726898193</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
@@ -9336,16 +9492,16 @@
         <v>56</v>
       </c>
       <c r="B57">
-        <v>66.091461181640597</v>
+        <v>66.323165893554602</v>
       </c>
       <c r="C57">
-        <v>25.784431457519499</v>
+        <v>25.778444290161101</v>
       </c>
       <c r="D57">
-        <v>0.41825512051582298</v>
+        <v>0.42646184563636702</v>
       </c>
       <c r="E57">
-        <v>3.17988061904907</v>
+        <v>2.8232669830322199</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
@@ -9353,16 +9509,16 @@
         <v>57</v>
       </c>
       <c r="B58">
-        <v>66.189018249511705</v>
+        <v>66.402435302734304</v>
       </c>
       <c r="C58">
-        <v>26.065868377685501</v>
+        <v>27.143712997436499</v>
       </c>
       <c r="D58">
-        <v>0.42555895447731001</v>
+        <v>0.43039157986640902</v>
       </c>
       <c r="E58">
-        <v>2.8166084289550701</v>
+        <v>2.6754808425903298</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
@@ -9370,16 +9526,16 @@
         <v>58</v>
       </c>
       <c r="B59">
-        <v>67.475608825683594</v>
+        <v>64.664634704589801</v>
       </c>
       <c r="C59">
-        <v>25.5269470214843</v>
+        <v>25.467067718505799</v>
       </c>
       <c r="D59">
-        <v>0.41996848583221402</v>
+        <v>0.42645156383514399</v>
       </c>
       <c r="E59">
-        <v>3.2224857807159402</v>
+        <v>2.96368408203125</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
@@ -9387,16 +9543,16 @@
         <v>59</v>
       </c>
       <c r="B60">
-        <v>66.451217651367102</v>
+        <v>67.585365295410099</v>
       </c>
       <c r="C60">
-        <v>25.479042053222599</v>
+        <v>24.994012832641602</v>
       </c>
       <c r="D60">
-        <v>0.42698043584823597</v>
+        <v>0.41407436132431003</v>
       </c>
       <c r="E60">
-        <v>3.1208035945892298</v>
+        <v>3.5480098724365199</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
@@ -9404,16 +9560,16 @@
         <v>60</v>
       </c>
       <c r="B61">
-        <v>66.993896484375</v>
+        <v>65.713409423828097</v>
       </c>
       <c r="C61">
-        <v>26.3592815399169</v>
+        <v>25.856288909912099</v>
       </c>
       <c r="D61">
-        <v>0.41242799162864602</v>
+        <v>0.42035239934921198</v>
       </c>
       <c r="E61">
-        <v>2.7621810436248699</v>
+        <v>3.1242403984069802</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
@@ -9421,16 +9577,16 @@
         <v>61</v>
       </c>
       <c r="B62">
-        <v>66.908531188964801</v>
+        <v>66.518287658691406</v>
       </c>
       <c r="C62">
-        <v>24.7305393218994</v>
+        <v>24.658683776855401</v>
       </c>
       <c r="D62">
-        <v>0.40616500377655002</v>
+        <v>0.41605004668235701</v>
       </c>
       <c r="E62">
-        <v>3.5387775897979701</v>
+        <v>3.8070909976959202</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
@@ -9438,16 +9594,16 @@
         <v>62</v>
       </c>
       <c r="B63">
-        <v>67.725608825683594</v>
+        <v>67.060974121093693</v>
       </c>
       <c r="C63">
-        <v>25.3053894042968</v>
+        <v>25.083833694458001</v>
       </c>
       <c r="D63">
-        <v>0.40202873945236201</v>
+        <v>0.40703579783439597</v>
       </c>
       <c r="E63">
-        <v>3.3482594490051198</v>
+        <v>3.4684653282165501</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
@@ -9455,16 +9611,16 @@
         <v>63</v>
       </c>
       <c r="B64">
-        <v>67.689018249511705</v>
+        <v>67.628044128417898</v>
       </c>
       <c r="C64">
-        <v>25.371257781982401</v>
+        <v>24.784431457519499</v>
       </c>
       <c r="D64">
-        <v>0.40690779685974099</v>
+        <v>0.401586323976516</v>
       </c>
       <c r="E64">
-        <v>3.6750752925872798</v>
+        <v>3.5887901782989502</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
@@ -9472,16 +9628,458 @@
         <v>64</v>
       </c>
       <c r="B65">
-        <v>68.682922363281193</v>
+        <v>66.939018249511705</v>
       </c>
       <c r="C65">
-        <v>25.215570449829102</v>
+        <v>25.2395210266113</v>
       </c>
       <c r="D65">
-        <v>0.401779115200042</v>
+        <v>0.41212663054466198</v>
       </c>
       <c r="E65">
-        <v>4.0025038719177202</v>
+        <v>3.3366835117339999</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66">
+        <v>67.25</v>
+      </c>
+      <c r="C66">
+        <v>25.3053894042968</v>
+      </c>
+      <c r="D66">
+        <v>0.40616419911384499</v>
+      </c>
+      <c r="E66">
+        <v>3.1462512016296298</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67">
+        <v>68.201217651367102</v>
+      </c>
+      <c r="C67">
+        <v>25.712575912475501</v>
+      </c>
+      <c r="D67">
+        <v>0.40472224354743902</v>
+      </c>
+      <c r="E67">
+        <v>3.5440466403961102</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68">
+        <v>68.689018249511705</v>
+      </c>
+      <c r="C68">
+        <v>24.910181045532202</v>
+      </c>
+      <c r="D68">
+        <v>0.39919036626815702</v>
+      </c>
+      <c r="E68">
+        <v>3.2894613742828298</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69">
+        <v>69.896339416503906</v>
+      </c>
+      <c r="C69">
+        <v>24.760480880737301</v>
+      </c>
+      <c r="D69">
+        <v>0.38850584626197798</v>
+      </c>
+      <c r="E69">
+        <v>3.6034970283508301</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70">
+        <v>70.353652954101506</v>
+      </c>
+      <c r="C70">
+        <v>25.1736545562744</v>
+      </c>
+      <c r="D70">
+        <v>0.38469231128692599</v>
+      </c>
+      <c r="E70">
+        <v>3.3981032371520898</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>70</v>
+      </c>
+      <c r="B71">
+        <v>70.560974121093693</v>
+      </c>
+      <c r="C71">
+        <v>24.796407699584901</v>
+      </c>
+      <c r="D71">
+        <v>0.37821093201637201</v>
+      </c>
+      <c r="E71">
+        <v>3.4557404518127401</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>71</v>
+      </c>
+      <c r="B72">
+        <v>70.012191772460895</v>
+      </c>
+      <c r="C72">
+        <v>24.497007369995099</v>
+      </c>
+      <c r="D72">
+        <v>0.380923271179199</v>
+      </c>
+      <c r="E72">
+        <v>4.3002834320068297</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>72</v>
+      </c>
+      <c r="B73">
+        <v>70.963409423828097</v>
+      </c>
+      <c r="C73">
+        <v>24.688623428344702</v>
+      </c>
+      <c r="D73">
+        <v>0.37189233303070002</v>
+      </c>
+      <c r="E73">
+        <v>4.2543582916259703</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>73</v>
+      </c>
+      <c r="B74">
+        <v>70.317070007324205</v>
+      </c>
+      <c r="C74">
+        <v>24.964073181152301</v>
+      </c>
+      <c r="D74">
+        <v>0.38029175996780301</v>
+      </c>
+      <c r="E74">
+        <v>4.2165532112121502</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>74</v>
+      </c>
+      <c r="B75">
+        <v>70.408531188964801</v>
+      </c>
+      <c r="C75">
+        <v>27.556886672973601</v>
+      </c>
+      <c r="D75">
+        <v>0.38084781169891302</v>
+      </c>
+      <c r="E75">
+        <v>3.3583178520202601</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>75</v>
+      </c>
+      <c r="B76">
+        <v>72.243896484375</v>
+      </c>
+      <c r="C76">
+        <v>25.904191970825099</v>
+      </c>
+      <c r="D76">
+        <v>0.36228969693183899</v>
+      </c>
+      <c r="E76">
+        <v>3.7013142108917201</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>76</v>
+      </c>
+      <c r="B77">
+        <v>71.189018249511705</v>
+      </c>
+      <c r="C77">
+        <v>25.850299835205</v>
+      </c>
+      <c r="D77">
+        <v>0.36639520525932301</v>
+      </c>
+      <c r="E77">
+        <v>3.07607698440551</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>77</v>
+      </c>
+      <c r="B78">
+        <v>72.262191772460895</v>
+      </c>
+      <c r="C78">
+        <v>26.179641723632798</v>
+      </c>
+      <c r="D78">
+        <v>0.35581195354461598</v>
+      </c>
+      <c r="E78">
+        <v>3.7898185253143302</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>78</v>
+      </c>
+      <c r="B79">
+        <v>71.579269409179602</v>
+      </c>
+      <c r="C79">
+        <v>27.131736755371001</v>
+      </c>
+      <c r="D79">
+        <v>0.36371639370918202</v>
+      </c>
+      <c r="E79">
+        <v>3.63780665397644</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>79</v>
+      </c>
+      <c r="B80">
+        <v>72.695121765136705</v>
+      </c>
+      <c r="C80">
+        <v>25.125749588012599</v>
+      </c>
+      <c r="D80">
+        <v>0.35690340399742099</v>
+      </c>
+      <c r="E80">
+        <v>4.1664080619812003</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>80</v>
+      </c>
+      <c r="B81">
+        <v>71.524391174316406</v>
+      </c>
+      <c r="C81">
+        <v>25.856288909912099</v>
+      </c>
+      <c r="D81">
+        <v>0.35974159836769098</v>
+      </c>
+      <c r="E81">
+        <v>3.85595273971557</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <v>81</v>
+      </c>
+      <c r="B82">
+        <v>72.292678833007798</v>
+      </c>
+      <c r="C82">
+        <v>26.011976242065401</v>
+      </c>
+      <c r="D82">
+        <v>0.35746476054191501</v>
+      </c>
+      <c r="E82">
+        <v>3.75832748413085</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>82</v>
+      </c>
+      <c r="B83">
+        <v>72.164634704589801</v>
+      </c>
+      <c r="C83">
+        <v>25.0359287261962</v>
+      </c>
+      <c r="D83">
+        <v>0.35489431023597701</v>
+      </c>
+      <c r="E83">
+        <v>3.8929359912872301</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A84">
+        <v>83</v>
+      </c>
+      <c r="B84">
+        <v>72.274391174316406</v>
+      </c>
+      <c r="C84">
+        <v>26.1556892395019</v>
+      </c>
+      <c r="D84">
+        <v>0.35309934616088801</v>
+      </c>
+      <c r="E84">
+        <v>4.4235644340515101</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A85">
+        <v>84</v>
+      </c>
+      <c r="B85">
+        <v>73.628044128417898</v>
+      </c>
+      <c r="C85">
+        <v>25.0538940429687</v>
+      </c>
+      <c r="D85">
+        <v>0.34767031669616699</v>
+      </c>
+      <c r="E85">
+        <v>4.74015140533447</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A86">
+        <v>85</v>
+      </c>
+      <c r="B86">
+        <v>72.091461181640597</v>
+      </c>
+      <c r="C86">
+        <v>25.497007369995099</v>
+      </c>
+      <c r="D86">
+        <v>0.35064059495925898</v>
+      </c>
+      <c r="E86">
+        <v>4.2916960716247496</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A87">
+        <v>86</v>
+      </c>
+      <c r="B87">
+        <v>73.347557067871094</v>
+      </c>
+      <c r="C87">
+        <v>24.293413162231399</v>
+      </c>
+      <c r="D87">
+        <v>0.34868332743644698</v>
+      </c>
+      <c r="E87">
+        <v>3.8454051017761199</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <v>87</v>
+      </c>
+      <c r="B88">
+        <v>72.487800598144503</v>
+      </c>
+      <c r="C88">
+        <v>26.772455215454102</v>
+      </c>
+      <c r="D88">
+        <v>0.34937772154808</v>
+      </c>
+      <c r="E88">
+        <v>4.1016278266906703</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A89">
+        <v>88</v>
+      </c>
+      <c r="B89">
+        <v>73.109756469726506</v>
+      </c>
+      <c r="C89">
+        <v>25.8023967742919</v>
+      </c>
+      <c r="D89">
+        <v>0.35218340158462502</v>
+      </c>
+      <c r="E89">
+        <v>4.4023203849792401</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A90">
+        <v>89</v>
+      </c>
+      <c r="B90">
+        <v>73.664634704589801</v>
+      </c>
+      <c r="C90">
+        <v>27.179641723632798</v>
+      </c>
+      <c r="D90">
+        <v>0.342809438705444</v>
+      </c>
+      <c r="E90">
+        <v>4.2540831565856898</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A91">
+        <v>90</v>
+      </c>
+      <c r="B91">
+        <v>74.1219482421875</v>
+      </c>
+      <c r="C91">
+        <v>25.3413181304931</v>
+      </c>
+      <c r="D91">
+        <v>0.34317058324813798</v>
+      </c>
+      <c r="E91">
+        <v>4.61743068695068</v>
       </c>
     </row>
   </sheetData>
@@ -9493,7 +10091,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E557F5C6-F7C3-2A40-891D-96BA5F29E064}">
   <dimension ref="A1:E67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A51" workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
@@ -10648,7 +11246,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>